<commit_message>
Update utility & security scores so that 1/0 is the best/worst
</commit_message>
<xml_diff>
--- a/SmplResults/results_test.xlsx
+++ b/SmplResults/results_test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Dataset\PeopleFlowData_nightley\SampleProgram_20190613\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\Dataset\PeopleFlowData_nightley\SampleProgram_20190629\SmplResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCBFFBED-FAD8-4667-8CAD-C3BE828CDBD1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A39C9407-AF8A-4142-BE10-50BA1859102F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -844,7 +844,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -856,7 +856,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -903,13 +903,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.49825714285714201</c:v>
+                  <c:v>0.50174285714285705</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.80020000000000002</c:v>
+                  <c:v>0.19979999999999901</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95185714285714196</c:v>
+                  <c:v>4.8142857142857098E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -921,13 +921,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98399999999999999</c:v>
+                  <c:v>1.6E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.371</c:v>
+                  <c:v>0.629</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -974,22 +974,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.29367977756140801</c:v>
+                  <c:v>0.70632022243859205</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.645608873536061</c:v>
+                  <c:v>0.354391126463938</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85887721955685004</c:v>
+                  <c:v>0.14112278044314899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.655319197004952</c:v>
+                  <c:v>0.344680802995047</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.82691098873935098</c:v>
+                  <c:v>0.17308901126064799</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.93093914678132395</c:v>
+                  <c:v>6.9060853218675805E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1001,22 +1001,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95099999999999996</c:v>
+                  <c:v>4.9000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79700000000000004</c:v>
+                  <c:v>0.191999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55200000000000005</c:v>
+                  <c:v>0.45099999999999901</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.245</c:v>
+                  <c:v>0.745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1063,31 +1063,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.99126080857444998</c:v>
+                  <c:v>8.7391914255493496E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99119899310833604</c:v>
+                  <c:v>8.8010068916630699E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98964829992144299</c:v>
+                  <c:v>1.0351700078556601E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98562553384748997</c:v>
+                  <c:v>1.43744661525091E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.97281935663048502</c:v>
+                  <c:v>2.7180643369514399E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.94185442398078401</c:v>
+                  <c:v>5.81455760192158E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.86617820054398897</c:v>
+                  <c:v>0.13382179945601</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.71078874193618002</c:v>
+                  <c:v>0.28921125806381898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.49809943541726098</c:v>
+                  <c:v>0.50190056458273802</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1099,31 +1099,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2E-3</c:v>
+                  <c:v>0.998</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94599999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.54600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.3999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.45400000000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.95399999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1170,31 +1170,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.99704605763526999</c:v>
+                  <c:v>2.9539423647296698E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.993689722905711</c:v>
+                  <c:v>6.3102770942886598E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.88101143836791596</c:v>
+                  <c:v>0.118988561632083</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.71616823804259699</c:v>
+                  <c:v>0.28383176195740201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.57424569828806304</c:v>
+                  <c:v>0.42575430171193601</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.461807126868019</c:v>
+                  <c:v>0.53819287313198005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.37909053546531402</c:v>
+                  <c:v>0.62090946453468499</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.31640669240296498</c:v>
+                  <c:v>0.68359330759703396</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.26929979736021997</c:v>
+                  <c:v>0.73070020263977897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1206,31 +1206,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1E-3</c:v>
+                  <c:v>0.999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1E-3</c:v>
+                  <c:v>0.999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3000000000000002E-2</c:v>
+                  <c:v>0.96699999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.221</c:v>
+                  <c:v>0.77900000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.53900000000000003</c:v>
+                  <c:v>0.46099999999999902</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.80700000000000005</c:v>
+                  <c:v>0.19299999999999901</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.91900000000000004</c:v>
+                  <c:v>8.0999999999999905E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.96599999999999997</c:v>
+                  <c:v>3.4000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.98899999999999999</c:v>
+                  <c:v>1.0999999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1277,7 +1277,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.98330293317658202</c:v>
+                  <c:v>1.6697066823417601E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1289,7 +1289,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1724,7 +1724,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1736,7 +1736,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1783,13 +1783,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.49825714285714201</c:v>
+                  <c:v>0.50174285714285705</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.80020000000000002</c:v>
+                  <c:v>0.19979999999999901</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95185714285714196</c:v>
+                  <c:v>4.8142857142857098E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1801,13 +1801,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.58276156786414401</c:v>
+                  <c:v>0.41723843213585499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32205334331255497</c:v>
+                  <c:v>0.67931311605810896</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17516312917724999</c:v>
+                  <c:v>0.82468042917114803</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1854,22 +1854,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.29367977756140801</c:v>
+                  <c:v>0.70632022243859205</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.645608873536061</c:v>
+                  <c:v>0.354391126463938</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85887721955685004</c:v>
+                  <c:v>0.14112278044314899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.655319197004952</c:v>
+                  <c:v>0.344680802995047</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.82691098873935098</c:v>
+                  <c:v>0.17308901126064799</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.93093914678132395</c:v>
+                  <c:v>6.9060853218675805E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1881,22 +1881,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.93058734549904798</c:v>
+                  <c:v>6.9412654500951798E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.547812705299495</c:v>
+                  <c:v>0.45218729470050401</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.30150837983798401</c:v>
+                  <c:v>0.70301300275451895</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.49669425618985902</c:v>
+                  <c:v>0.481266058716178</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.248130615673055</c:v>
+                  <c:v>0.74467538810767797</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.167078668653666</c:v>
+                  <c:v>0.82832413352055301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1943,31 +1943,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.99126080857444998</c:v>
+                  <c:v>8.7391914255493496E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99119899310833604</c:v>
+                  <c:v>8.8010068916630699E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98964829992144299</c:v>
+                  <c:v>1.0351700078556601E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.98562553384748997</c:v>
+                  <c:v>1.43744661525091E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.97281935663048502</c:v>
+                  <c:v>2.7180643369514399E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.94185442398078401</c:v>
+                  <c:v>5.81455760192158E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.86617820054398897</c:v>
+                  <c:v>0.13382179945601</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.71078874193618002</c:v>
+                  <c:v>0.28921125806381898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.49809943541726098</c:v>
+                  <c:v>0.50190056458273802</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1979,31 +1979,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.4601666079431501E-2</c:v>
+                  <c:v>0.98456648806928804</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.46731708241769E-2</c:v>
+                  <c:v>0.98374348908880505</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6467181226789598E-2</c:v>
+                  <c:v>0.98370707523744205</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.55144929107351E-2</c:v>
+                  <c:v>0.98446194134402198</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5785312148649901E-2</c:v>
+                  <c:v>0.98418133991453505</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0700829516549599E-2</c:v>
+                  <c:v>0.97940888281467697</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.4173009317328306E-2</c:v>
+                  <c:v>0.93639521118326297</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25863629607462202</c:v>
+                  <c:v>0.73732764313614896</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.50190056458273802</c:v>
+                  <c:v>0.49809943541726098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2050,31 +2050,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.99704605763526999</c:v>
+                  <c:v>2.9539423647296698E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.993689722905711</c:v>
+                  <c:v>6.3102770942886598E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.88101143836791596</c:v>
+                  <c:v>0.118988561632083</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.71616823804259699</c:v>
+                  <c:v>0.28383176195740201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.57424569828806304</c:v>
+                  <c:v>0.42575430171193601</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.461807126868019</c:v>
+                  <c:v>0.53819287313198005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.37909053546531402</c:v>
+                  <c:v>0.62090946453468499</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.31640669240296498</c:v>
+                  <c:v>0.68359330759703396</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.26929979736021997</c:v>
+                  <c:v>0.73070020263977897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2086,31 +2086,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4.52665558886408E-3</c:v>
+                  <c:v>0.99528621966834097</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.8635333455443403E-3</c:v>
+                  <c:v>0.99267666096663498</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4303169172591E-2</c:v>
+                  <c:v>0.97574602634457597</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.8798486010507295E-2</c:v>
+                  <c:v>0.92784541953017996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.19917034182962001</c:v>
+                  <c:v>0.81299722818411602</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.36250877744894699</c:v>
+                  <c:v>0.62670036027286002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.51198995640027001</c:v>
+                  <c:v>0.49180584575644698</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.63214771405418901</c:v>
+                  <c:v>0.37590086416142898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.71516661734216103</c:v>
+                  <c:v>0.298298897436377</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2157,7 +2157,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.98330293317658202</c:v>
+                  <c:v>1.6697066823417601E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2169,7 +2169,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2604,7 +2604,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2616,7 +2616,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2663,13 +2663,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.98399999999999999</c:v>
+                  <c:v>1.6E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.371</c:v>
+                  <c:v>0.629</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2681,13 +2681,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.58276156786414401</c:v>
+                  <c:v>0.41723843213585499</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32205334331255497</c:v>
+                  <c:v>0.67931311605810896</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17516312917724999</c:v>
+                  <c:v>0.82468042917114803</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2734,22 +2734,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95099999999999996</c:v>
+                  <c:v>4.9000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79700000000000004</c:v>
+                  <c:v>0.191999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55200000000000005</c:v>
+                  <c:v>0.45099999999999901</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.245</c:v>
+                  <c:v>0.745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2761,22 +2761,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.93058734549904798</c:v>
+                  <c:v>6.9412654500951798E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.547812705299495</c:v>
+                  <c:v>0.45218729470050401</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.30150837983798401</c:v>
+                  <c:v>0.70301300275451895</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.49669425618985902</c:v>
+                  <c:v>0.481266058716178</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.248130615673055</c:v>
+                  <c:v>0.74467538810767797</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.167078668653666</c:v>
+                  <c:v>0.82832413352055301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2823,31 +2823,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2E-3</c:v>
+                  <c:v>0.998</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94599999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.54600000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.3999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.45400000000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.95399999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2859,31 +2859,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.4601666079431501E-2</c:v>
+                  <c:v>0.98456648806928804</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.46731708241769E-2</c:v>
+                  <c:v>0.98374348908880505</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6467181226789598E-2</c:v>
+                  <c:v>0.98370707523744205</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.55144929107351E-2</c:v>
+                  <c:v>0.98446194134402198</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5785312148649901E-2</c:v>
+                  <c:v>0.98418133991453505</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0700829516549599E-2</c:v>
+                  <c:v>0.97940888281467697</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.4173009317328306E-2</c:v>
+                  <c:v>0.93639521118326297</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25863629607462202</c:v>
+                  <c:v>0.73732764313614896</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.50190056458273802</c:v>
+                  <c:v>0.49809943541726098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2930,31 +2930,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1E-3</c:v>
+                  <c:v>0.999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1E-3</c:v>
+                  <c:v>0.999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.3000000000000002E-2</c:v>
+                  <c:v>0.96699999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.221</c:v>
+                  <c:v>0.77900000000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.53900000000000003</c:v>
+                  <c:v>0.46099999999999902</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.80700000000000005</c:v>
+                  <c:v>0.19299999999999901</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.91900000000000004</c:v>
+                  <c:v>8.0999999999999905E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.96599999999999997</c:v>
+                  <c:v>3.4000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.98899999999999999</c:v>
+                  <c:v>1.0999999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2966,31 +2966,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4.52665558886408E-3</c:v>
+                  <c:v>0.99528621966834097</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.8635333455443403E-3</c:v>
+                  <c:v>0.99267666096663498</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4303169172591E-2</c:v>
+                  <c:v>0.97574602634457597</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.8798486010507295E-2</c:v>
+                  <c:v>0.92784541953017996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.19917034182962001</c:v>
+                  <c:v>0.81299722818411602</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.36250877744894699</c:v>
+                  <c:v>0.62670036027286002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.51198995640027001</c:v>
+                  <c:v>0.49180584575644698</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.63214771405418901</c:v>
+                  <c:v>0.37590086416142898</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.71516661734216103</c:v>
+                  <c:v>0.298298897436377</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3037,7 +3037,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3049,7 +3049,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5507,11 +5507,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="11.4140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
@@ -5538,19 +5539,19 @@
         <v>6</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0.999</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
       <c r="E2">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5558,19 +5559,19 @@
         <v>7</v>
       </c>
       <c r="B3">
-        <v>0.49825714285714201</v>
+        <v>0.50174285714285705</v>
       </c>
       <c r="C3">
-        <v>1E-3</v>
+        <v>0.999</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F3">
-        <v>0.58276156786414401</v>
+        <v>0.41723843213585499</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5578,19 +5579,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.80020000000000002</v>
+        <v>0.19979999999999901</v>
       </c>
       <c r="C4">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0.98399999999999999</v>
+        <v>1.6E-2</v>
       </c>
       <c r="E4">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F4">
-        <v>0.32205334331255497</v>
+        <v>0.67931311605810896</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5598,19 +5599,19 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <v>0.95185714285714196</v>
+        <v>4.8142857142857098E-2</v>
       </c>
       <c r="C5">
-        <v>2E-3</v>
+        <v>0.999</v>
       </c>
       <c r="D5">
-        <v>0.371</v>
+        <v>0.629</v>
       </c>
       <c r="E5">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F5">
-        <v>0.17516312917724999</v>
+        <v>0.82468042917114803</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5618,19 +5619,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.29367977756140801</v>
+        <v>0.70632022243859205</v>
       </c>
       <c r="C6">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F6">
-        <v>0.93058734549904798</v>
+        <v>6.9412654500951798E-2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5638,19 +5639,19 @@
         <v>11</v>
       </c>
       <c r="B7">
-        <v>0.645608873536061</v>
+        <v>0.354391126463938</v>
       </c>
       <c r="C7">
-        <v>1E-3</v>
+        <v>0.999</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F7">
-        <v>0.547812705299495</v>
+        <v>0.45218729470050401</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5658,19 +5659,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.85887721955685004</v>
+        <v>0.14112278044314899</v>
       </c>
       <c r="C8">
-        <v>3.0000000000000001E-3</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0.95099999999999996</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="E8">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F8">
-        <v>0.30150837983798401</v>
+        <v>0.70301300275451895</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5678,19 +5679,19 @@
         <v>13</v>
       </c>
       <c r="B9">
-        <v>0.655319197004952</v>
+        <v>0.344680802995047</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.999</v>
       </c>
       <c r="D9">
-        <v>0.79700000000000004</v>
+        <v>0.191999999999999</v>
       </c>
       <c r="E9">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F9">
-        <v>0.49669425618985902</v>
+        <v>0.481266058716178</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5698,19 +5699,19 @@
         <v>14</v>
       </c>
       <c r="B10">
-        <v>0.82691098873935098</v>
+        <v>0.17308901126064799</v>
       </c>
       <c r="C10">
-        <v>1E-3</v>
+        <v>0.997</v>
       </c>
       <c r="D10">
-        <v>0.55200000000000005</v>
+        <v>0.45099999999999901</v>
       </c>
       <c r="E10">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F10">
-        <v>0.248130615673055</v>
+        <v>0.74467538810767797</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5718,19 +5719,19 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>0.93093914678132395</v>
+        <v>6.9060853218675805E-2</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.999</v>
       </c>
       <c r="D11">
-        <v>0.245</v>
+        <v>0.745</v>
       </c>
       <c r="E11">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F11">
-        <v>0.167078668653666</v>
+        <v>0.82832413352055301</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5738,19 +5739,19 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>0.99126080857444998</v>
+        <v>8.7391914255493496E-3</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.999</v>
       </c>
       <c r="D12">
-        <v>2E-3</v>
+        <v>0.998</v>
       </c>
       <c r="E12">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F12">
-        <v>1.4601666079431501E-2</v>
+        <v>0.98456648806928804</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5758,19 +5759,19 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>0.99119899310833604</v>
+        <v>8.8010068916630699E-3</v>
       </c>
       <c r="C13">
-        <v>1E-3</v>
+        <v>0.998</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F13">
-        <v>1.46731708241769E-2</v>
+        <v>0.98374348908880505</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5778,19 +5779,19 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>0.98964829992144299</v>
+        <v>1.0351700078556601E-2</v>
       </c>
       <c r="C14">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F14">
-        <v>1.6467181226789598E-2</v>
+        <v>0.98370707523744205</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5798,19 +5799,19 @@
         <v>19</v>
       </c>
       <c r="B15">
-        <v>0.98562553384748997</v>
+        <v>1.43744661525091E-2</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>4.0000000000000001E-3</v>
+        <v>0.996</v>
       </c>
       <c r="E15">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F15">
-        <v>1.55144929107351E-2</v>
+        <v>0.98446194134402198</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5818,19 +5819,19 @@
         <v>20</v>
       </c>
       <c r="B16">
-        <v>0.97281935663048502</v>
+        <v>2.7180643369514399E-2</v>
       </c>
       <c r="C16">
-        <v>2E-3</v>
+        <v>0.999</v>
       </c>
       <c r="D16">
-        <v>5.0000000000000001E-3</v>
+        <v>0.995</v>
       </c>
       <c r="E16">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F16">
-        <v>1.5785312148649901E-2</v>
+        <v>0.98418133991453505</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5838,19 +5839,19 @@
         <v>21</v>
       </c>
       <c r="B17">
-        <v>0.94185442398078401</v>
+        <v>5.81455760192158E-2</v>
       </c>
       <c r="C17">
-        <v>2E-3</v>
+        <v>0.996</v>
       </c>
       <c r="D17">
-        <v>5.3999999999999999E-2</v>
+        <v>0.94599999999999995</v>
       </c>
       <c r="E17">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F17">
-        <v>2.0700829516549599E-2</v>
+        <v>0.97940888281467697</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5858,19 +5859,19 @@
         <v>22</v>
       </c>
       <c r="B18">
-        <v>0.86617820054398897</v>
+        <v>0.13382179945601</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <v>0.45400000000000001</v>
+        <v>0.54600000000000004</v>
       </c>
       <c r="E18">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F18">
-        <v>6.4173009317328306E-2</v>
+        <v>0.93639521118326297</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5878,19 +5879,19 @@
         <v>23</v>
       </c>
       <c r="B19">
-        <v>0.71078874193618002</v>
+        <v>0.28921125806381898</v>
       </c>
       <c r="C19">
-        <v>2E-3</v>
+        <v>0.999</v>
       </c>
       <c r="D19">
-        <v>0.95399999999999996</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="E19">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F19">
-        <v>0.25863629607462202</v>
+        <v>0.73732764313614896</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5898,19 +5899,19 @@
         <v>24</v>
       </c>
       <c r="B20">
+        <v>0.50190056458273802</v>
+      </c>
+      <c r="C20">
+        <v>0.999</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0.99131178743725901</v>
+      </c>
+      <c r="F20">
         <v>0.49809943541726098</v>
-      </c>
-      <c r="C20">
-        <v>1E-3</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>8.68821256274095E-3</v>
-      </c>
-      <c r="F20">
-        <v>0.50190056458273802</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5918,19 +5919,19 @@
         <v>25</v>
       </c>
       <c r="B21">
-        <v>0.99704605763526999</v>
+        <v>2.9539423647296698E-3</v>
       </c>
       <c r="C21">
-        <v>2E-3</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <v>1E-3</v>
+        <v>0.999</v>
       </c>
       <c r="E21">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F21">
-        <v>4.52665558886408E-3</v>
+        <v>0.99528621966834097</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5938,19 +5939,19 @@
         <v>26</v>
       </c>
       <c r="B22">
-        <v>0.993689722905711</v>
+        <v>6.3102770942886598E-3</v>
       </c>
       <c r="C22">
-        <v>1E-3</v>
+        <v>0.999</v>
       </c>
       <c r="D22">
-        <v>1E-3</v>
+        <v>0.999</v>
       </c>
       <c r="E22">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F22">
-        <v>7.8635333455443403E-3</v>
+        <v>0.99267666096663498</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5958,19 +5959,19 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>0.88101143836791596</v>
+        <v>0.118988561632083</v>
       </c>
       <c r="C23">
-        <v>2E-3</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>3.3000000000000002E-2</v>
+        <v>0.96699999999999997</v>
       </c>
       <c r="E23">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F23">
-        <v>2.4303169172591E-2</v>
+        <v>0.97574602634457597</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5978,19 +5979,19 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>0.71616823804259699</v>
+        <v>0.28383176195740201</v>
       </c>
       <c r="C24">
-        <v>1E-3</v>
+        <v>0.998</v>
       </c>
       <c r="D24">
-        <v>0.221</v>
+        <v>0.77900000000000003</v>
       </c>
       <c r="E24">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F24">
-        <v>6.8798486010507295E-2</v>
+        <v>0.92784541953017996</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5998,19 +5999,19 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>0.57424569828806304</v>
+        <v>0.42575430171193601</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>0.999</v>
       </c>
       <c r="D25">
-        <v>0.53900000000000003</v>
+        <v>0.46099999999999902</v>
       </c>
       <c r="E25">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F25">
-        <v>0.19917034182962001</v>
+        <v>0.81299722818411602</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -6018,19 +6019,19 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>0.461807126868019</v>
+        <v>0.53819287313198005</v>
       </c>
       <c r="C26">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>0.80700000000000005</v>
+        <v>0.19299999999999901</v>
       </c>
       <c r="E26">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F26">
-        <v>0.36250877744894699</v>
+        <v>0.62670036027286002</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -6038,19 +6039,19 @@
         <v>31</v>
       </c>
       <c r="B27">
-        <v>0.37909053546531402</v>
+        <v>0.62090946453468499</v>
       </c>
       <c r="C27">
-        <v>2E-3</v>
+        <v>0.999</v>
       </c>
       <c r="D27">
-        <v>0.91900000000000004</v>
+        <v>8.0999999999999905E-2</v>
       </c>
       <c r="E27">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F27">
-        <v>0.51198995640027001</v>
+        <v>0.49180584575644698</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -6058,19 +6059,19 @@
         <v>32</v>
       </c>
       <c r="B28">
-        <v>0.31640669240296498</v>
+        <v>0.68359330759703396</v>
       </c>
       <c r="C28">
-        <v>5.0000000000000001E-3</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <v>0.96599999999999997</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="E28">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F28">
-        <v>0.63214771405418901</v>
+        <v>0.37590086416142898</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -6078,19 +6079,19 @@
         <v>33</v>
       </c>
       <c r="B29">
-        <v>0.26929979736021997</v>
+        <v>0.73070020263977897</v>
       </c>
       <c r="C29">
-        <v>1E-3</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <v>0.98899999999999999</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="E29">
-        <v>8.68821256274095E-3</v>
+        <v>0.99131178743725901</v>
       </c>
       <c r="F29">
-        <v>0.71516661734216103</v>
+        <v>0.298298897436377</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -6098,19 +6099,19 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <v>0.98330293317658202</v>
+        <v>1.6697066823417601E-2</v>
       </c>
       <c r="C30">
+        <v>0.998</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0.99131178743725901</v>
+      </c>
+      <c r="F30">
         <v>0</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>8.68821256274095E-3</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>